<commit_message>
python read and control Excel. Next Step: Send email from Python
</commit_message>
<xml_diff>
--- a/DailyReport_STECH.xlsx
+++ b/DailyReport_STECH.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2. To chu SI\2020\DailyReportAuto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoang\github\ExelReportHelper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51ABE14-DEA5-40CE-9E37-7F3DC6BB1EC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoangnph" sheetId="6" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <sheet name="TúNA" sheetId="5" r:id="rId6"/>
     <sheet name="AutoDailyReport" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -260,7 +259,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]h:mm\ AM/PM;@"/>
@@ -721,7 +720,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21F55E66-4CF8-40A9-9F26-04F53E182F9D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G39"/>
   <sheetViews>
@@ -1196,11 +1195,11 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1" xr:uid="{50AEC010-AFB3-4340-A778-FDD5CDF02728}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1">
       <formula1>43466</formula1>
       <formula2>47484</formula2>
     </dataValidation>
-    <dataValidation type="date" showInputMessage="1" showErrorMessage="1" sqref="A3:A9" xr:uid="{89D73067-238F-49B1-B3BD-A8447743029F}">
+    <dataValidation type="date" showInputMessage="1" showErrorMessage="1" sqref="A3:A9">
       <formula1>43466</formula1>
       <formula2>47484</formula2>
     </dataValidation>
@@ -1210,7 +1209,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G38"/>
   <sheetViews>
@@ -1608,7 +1607,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{343857D8-3A4B-4009-8B3C-14E7D3773274}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G38"/>
   <sheetViews>
@@ -2006,7 +2005,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EA40149-3D29-4623-81CD-0D1E7885592F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G38"/>
   <sheetViews>
@@ -2404,7 +2403,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE27295-FD14-4A25-9B57-A2DBE2795BE2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:G38"/>
   <sheetViews>
@@ -2802,7 +2801,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C27300-1F6E-4349-AA5E-AA4C86475E3B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:G38"/>
   <sheetViews>
@@ -3200,7 +3199,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AC571D2-6481-4D28-95EC-A6C00DDF0FA7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:P16"/>
   <sheetViews>

</xml_diff>

<commit_message>
Check sendmail with google
</commit_message>
<xml_diff>
--- a/DailyReport_STECH.xlsx
+++ b/DailyReport_STECH.xlsx
@@ -14,8 +14,8 @@
   <sheets>
     <sheet name="Hoangnph" sheetId="6" r:id="rId1"/>
     <sheet name="TrungTM" sheetId="1" r:id="rId2"/>
-    <sheet name="ĐứcNC" sheetId="2" r:id="rId3"/>
-    <sheet name="LuânPT" sheetId="3" r:id="rId4"/>
+    <sheet name="LuânPT" sheetId="3" r:id="rId3"/>
+    <sheet name="ĐứcNC" sheetId="2" r:id="rId4"/>
     <sheet name="HạnhDD" sheetId="4" r:id="rId5"/>
     <sheet name="TúNA" sheetId="5" r:id="rId6"/>
     <sheet name="AutoDailyReport" sheetId="7" r:id="rId7"/>
@@ -725,8 +725,8 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1608,7 +1608,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3"/>
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2006,11 +2006,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet4"/>
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>